<commit_message>
Extended Test Plan Breakdown
</commit_message>
<xml_diff>
--- a/Excel sheets/Examples/Chapter 06/LookupValue Test Plan breakdown - first stage.xlsx
+++ b/Excel sheets/Examples/Chapter 06/LookupValue Test Plan breakdown - first stage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2a63c87061b9b9b/Projects/Books/Automated Testing in Microsoft Dynamics 365 Business Central/2nd Edition/Source/Book/WORD/Chapter 6 - In Progress/Test Plan ^0 Test Design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\Examples\Chapter 06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{BAE623AF-B4E1-49DD-847F-1E777F18503D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5E0D0CC1-34F4-4C3A-8CD4-B89EFCF2C864}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EA8D8E-F2D3-402F-940A-7DD5850637DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21930" yWindow="3060" windowWidth="12615" windowHeight="6645" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="31635" yWindow="4140" windowWidth="12630" windowHeight="6675" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan breakdown" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>Feature</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Report</t>
+  </si>
+  <si>
+    <t>Permissions</t>
+  </si>
+  <si>
+    <t>Copy Document</t>
   </si>
 </sst>
 </file>
@@ -138,8 +144,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:B9" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:B9" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:B11" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:B11" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
@@ -445,9 +451,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -527,6 +535,22 @@
         <v>11</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>